<commit_message>
run the bad people :-)
</commit_message>
<xml_diff>
--- a/res/result.xlsx
+++ b/res/result.xlsx
@@ -1,63 +1,37 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20338"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\PycharmProjects\FB_GNN(latest)\res\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24ADB42F-D662-41D6-9E3E-5494EF299A2E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <workbookProtection/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="11520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
-  <si>
-    <t>people</t>
-  </si>
-  <si>
-    <t>2 Experts</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="2">
     <font>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <color theme="1"/>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <name val="宋体"/>
-      <family val="3"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <name val="宋体"/>
-      <family val="3"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
+      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -72,43 +46,93 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="1" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -396,358 +420,362 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:C31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
-  <cols>
-    <col min="3" max="3" width="11" customWidth="1"/>
-  </cols>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="B1" s="1" t="s">
+    <row r="1">
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>people</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>2 Experts</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="B2" t="n">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A2" s="1">
-        <v>0</v>
-      </c>
-      <c r="B2">
+      <c r="C2" t="n">
+        <v>0.3893</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="C2">
-        <v>0.38929999999999998</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A3" s="1">
-        <v>1</v>
-      </c>
-      <c r="B3">
+      <c r="B3" t="n">
         <v>2</v>
       </c>
-      <c r="C3">
-        <v>0.40710000000000002</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A4" s="1">
+      <c r="C3" t="n">
+        <v>0.4071</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="B4">
+      <c r="B4" t="n">
         <v>3</v>
       </c>
-      <c r="C4">
-        <v>0.34639999999999999</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A5" s="1">
+      <c r="C4" t="n">
+        <v>0.3464</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="B5">
+      <c r="B5" t="n">
         <v>4</v>
       </c>
-      <c r="C5">
-        <v>0.41189999999999999</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A6" s="1">
+      <c r="C5" t="n">
+        <v>0.4155</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="B6">
+      <c r="B6" t="n">
         <v>5</v>
       </c>
-      <c r="C6">
-        <v>0.48930000000000001</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A7" s="1">
+      <c r="C6" t="n">
+        <v>0.4893</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="B7">
+      <c r="B7" t="n">
         <v>6</v>
       </c>
-      <c r="C7">
-        <v>0.44879999999999998</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A8" s="1">
+      <c r="C7" t="n">
+        <v>0.4488</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="B8">
+      <c r="B8" t="n">
         <v>7</v>
       </c>
-      <c r="C8">
-        <v>0.37259999999999999</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A9" s="1">
+      <c r="C8" t="n">
+        <v>0.3726</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="n">
         <v>7</v>
       </c>
-      <c r="B9">
+      <c r="B9" t="n">
         <v>8</v>
       </c>
-      <c r="C9">
+      <c r="C9" t="n">
         <v>0.3952</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A10" s="1">
+    <row r="10">
+      <c r="A10" s="1" t="n">
         <v>8</v>
       </c>
-      <c r="B10">
+      <c r="B10" t="n">
         <v>9</v>
       </c>
-      <c r="C10">
+      <c r="C10" t="n">
         <v>0.3821</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A11" s="1">
+    <row r="11">
+      <c r="A11" s="1" t="n">
         <v>9</v>
       </c>
-      <c r="B11">
+      <c r="B11" t="n">
         <v>10</v>
       </c>
-      <c r="C11">
+      <c r="C11" t="n">
         <v>0.3226</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A12" s="1">
+    <row r="12">
+      <c r="A12" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="B12">
+      <c r="B12" t="n">
         <v>11</v>
       </c>
-      <c r="C12">
-        <v>0.34050000000000002</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A13" s="1">
+      <c r="C12" t="n">
+        <v>0.3405</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="1" t="n">
         <v>11</v>
       </c>
-      <c r="B13">
+      <c r="B13" t="n">
         <v>12</v>
       </c>
-      <c r="C13">
-        <v>0.32500000000000001</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A14" s="1">
+      <c r="C13" t="n">
+        <v>0.325</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="1" t="n">
         <v>12</v>
       </c>
-      <c r="B14">
+      <c r="B14" t="n">
         <v>13</v>
       </c>
-      <c r="C14">
-        <v>0.36070000000000002</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A15" s="1">
+      <c r="C14" t="n">
+        <v>0.3607</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="1" t="n">
         <v>13</v>
       </c>
-      <c r="B15">
+      <c r="B15" t="n">
         <v>14</v>
       </c>
-      <c r="C15">
-        <v>0.30709999999999998</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A16" s="1">
+      <c r="C15" t="n">
+        <v>0.3071</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="1" t="n">
         <v>14</v>
       </c>
-      <c r="B16">
+      <c r="B16" t="n">
         <v>15</v>
       </c>
-      <c r="C16">
+      <c r="C16" t="n">
         <v>0.3548</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A17" s="1">
+    <row r="17">
+      <c r="A17" s="1" t="n">
         <v>15</v>
       </c>
-      <c r="B17">
+      <c r="B17" t="n">
         <v>16</v>
       </c>
-      <c r="C17">
-        <v>0.39400000000000002</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A18" s="1">
+      <c r="C17" t="n">
+        <v>0.394</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="1" t="n">
         <v>16</v>
       </c>
-      <c r="B18">
+      <c r="B18" t="n">
         <v>17</v>
       </c>
-      <c r="C18">
+      <c r="C18" t="n">
         <v>0.4405</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A19" s="1">
+    <row r="19">
+      <c r="A19" s="1" t="n">
         <v>17</v>
       </c>
-      <c r="B19">
+      <c r="B19" t="n">
         <v>18</v>
       </c>
-      <c r="C19">
-        <v>0.41789999999999999</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A20" s="1">
+      <c r="C19" t="n">
+        <v>0.4179</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="1" t="n">
         <v>18</v>
       </c>
-      <c r="B20">
+      <c r="B20" t="n">
         <v>19</v>
       </c>
-      <c r="C20">
-        <v>0.36309999999999998</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A21" s="1">
+      <c r="C20" t="n">
+        <v>0.3631</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="1" t="n">
         <v>19</v>
       </c>
-      <c r="B21">
+      <c r="B21" t="n">
         <v>20</v>
       </c>
-      <c r="C21">
+      <c r="C21" t="n">
         <v>0.4405</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A22" s="1">
+    <row r="22">
+      <c r="A22" s="1" t="n">
         <v>20</v>
       </c>
-      <c r="B22">
+      <c r="B22" t="n">
         <v>21</v>
       </c>
-      <c r="C22">
-        <v>0.33929999999999999</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A23" s="1">
+      <c r="C22" t="n">
+        <v>0.3393</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="1" t="n">
         <v>21</v>
       </c>
-      <c r="B23">
+      <c r="B23" t="n">
         <v>22</v>
       </c>
-      <c r="C23">
-        <v>0.35709999999999997</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A24" s="1">
+      <c r="C23" t="n">
+        <v>0.3571</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="1" t="n">
         <v>22</v>
       </c>
-      <c r="B24">
+      <c r="B24" t="n">
         <v>23</v>
       </c>
-      <c r="C24">
-        <v>0.45479999999999998</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A25" s="1">
+      <c r="C24" t="n">
+        <v>0.4548</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="1" t="n">
         <v>23</v>
       </c>
-      <c r="B25">
+      <c r="B25" t="n">
         <v>24</v>
       </c>
-      <c r="C25">
-        <v>0.39639999999999997</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A26" s="1">
+      <c r="C25" t="n">
+        <v>0.3964</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="1" t="n">
         <v>24</v>
       </c>
-      <c r="B26">
+      <c r="B26" t="n">
         <v>25</v>
       </c>
-      <c r="C26">
-        <v>0.34399999999999997</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A27" s="1">
+      <c r="C26" t="n">
+        <v>0.344</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="1" t="n">
         <v>25</v>
       </c>
-      <c r="B27">
+      <c r="B27" t="n">
         <v>26</v>
       </c>
-      <c r="C27">
+      <c r="C27" t="n">
         <v>0.3286</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A28" s="1">
+    <row r="28">
+      <c r="A28" s="1" t="n">
         <v>26</v>
       </c>
-      <c r="B28">
+      <c r="B28" t="n">
         <v>27</v>
       </c>
-      <c r="C28">
-        <v>0.26069999999999999</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A29" s="1">
+      <c r="C28" t="n">
+        <v>0.2607</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="1" t="n">
         <v>27</v>
       </c>
-      <c r="B29">
+      <c r="B29" t="n">
         <v>28</v>
       </c>
-      <c r="C29">
-        <v>0.39760000000000001</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A30" s="1">
+      <c r="C29" t="n">
+        <v>0.3976</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="1" t="n">
         <v>28</v>
       </c>
-      <c r="B30">
+      <c r="B30" t="n">
         <v>29</v>
       </c>
-      <c r="C30">
-        <v>0.39879999999999999</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A31" s="1">
+      <c r="C30" t="n">
+        <v>0.3988</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="1" t="n">
         <v>29</v>
       </c>
-      <c r="B31">
+      <c r="B31" t="n">
         <v>30</v>
       </c>
-      <c r="C31">
-        <v>0.32379999999999998</v>
+      <c r="C31" t="n">
+        <v>0.3238</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="2" type="noConversion"/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
 </file>
</xml_diff>